<commit_message>
Soporte Pantalla y Riego
Cambios:
-Se incluye soporte de pantalla TFT_eSPI
-Mejoras en la lectura de la configuracion del secuenciador
-Mejoras en la generacion del json de estado de la maquina de estados
</commit_message>
<xml_diff>
--- a/.mio/Particiones_ESP32_v2.xlsx
+++ b/.mio/Particiones_ESP32_v2.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlopezt\Documents\PlatformIO\Projects\Actuador-ESP32\.mio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D61053A-8D1F-4F78-A10A-280022872716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6836DE-4D01-4628-B4F2-5955A07092EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A52EA33D-BD66-4045-9139-39A15A538EC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{A52EA33D-BD66-4045-9139-39A15A538EC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="esquema con gargador" sheetId="2" r:id="rId1"/>
+    <sheet name="esquema con cargador" sheetId="2" r:id="rId1"/>
+    <sheet name="esquema con cargador y SPIFFS" sheetId="3" r:id="rId2"/>
+    <sheet name="esquema simetrico y SPIFFS" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="73">
   <si>
     <t>Flags</t>
   </si>
@@ -141,13 +143,127 @@
   </si>
   <si>
     <t>Por definicion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SubType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flags</t>
+  </si>
+  <si>
+    <t>0x009000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nvs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x009000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x005000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ota</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x00E000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x002000</t>
+  </si>
+  <si>
+    <t>0x010000</t>
+  </si>
+  <si>
+    <t>0x0E0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> app</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ota_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x010000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x0E0000</t>
+  </si>
+  <si>
+    <t>0x0F0000</t>
+  </si>
+  <si>
+    <t>0x303800</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ota_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x0F0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x303800</t>
+  </si>
+  <si>
+    <t>0x3F3800</t>
+  </si>
+  <si>
+    <t>0x00C800</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spiffs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x3F3800</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x00C800</t>
+  </si>
+  <si>
+    <t>Tamaño (kB)</t>
+  </si>
+  <si>
+    <t>Sobra (kB)</t>
+  </si>
+  <si>
+    <t>Calculados</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Cargador</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Ocupación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +285,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,8 +312,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -621,11 +756,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -666,6 +839,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,10 +878,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1001,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951BFC8B-84AC-47C7-AF9F-2926E2701612}">
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17:R22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,20 +1434,20 @@
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="62"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20"/>
@@ -1640,10 +1834,10 @@
       <c r="F22" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="str">
@@ -1667,10 +1861,10 @@
         <v>0x005000</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="str">
@@ -1694,10 +1888,10 @@
         <v>0x002000</v>
       </c>
       <c r="F24" s="14"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="str">
@@ -1721,10 +1915,10 @@
         <v>0x180000</v>
       </c>
       <c r="F25" s="14"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="str">
@@ -1748,10 +1942,10 @@
         <v>0x180000</v>
       </c>
       <c r="F26" s="14"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="str">
@@ -1775,10 +1969,10 @@
         <v>0x0F0000</v>
       </c>
       <c r="F27" s="14"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="str">
@@ -1802,10 +1996,10 @@
         <v/>
       </c>
       <c r="F28" s="14"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="46"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="str">
@@ -1829,132 +2023,132 @@
         <v/>
       </c>
       <c r="F29" s="17"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>+CONCATENATE(A22,", ",B22,", ",C22,", ",D22,", ",E22,", ",F22)</f>
         <v># Name, Type, SubType, Offset, Size, Flags</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" ref="A34:A40" si="10">+CONCATENATE(A23,", ",B23,", ",C23,", ",D23,", ",E23,", ",F23)</f>
         <v xml:space="preserve">nvs, data, nvs, 0x009000, 0x005000, </v>
       </c>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">otadata, data, ota, 0x00E000, 0x002000, </v>
       </c>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">Loader, app, ota_0, 0x010000, 0x180000, </v>
       </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">app, app, ota_1, 0x190000, 0x180000, </v>
       </c>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">spiffs, data, spiffs, 0x310000, 0x0F0000, </v>
       </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">, , , , , </v>
       </c>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
-      <c r="K39" s="46"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">, , , , , </v>
       </c>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
-      <c r="K40" s="46"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H43" s="46"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
-      <c r="K43" s="46"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1965,4 +2159,1996 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97B26DB-C23A-48BC-BF73-E8DD90832414}">
+  <dimension ref="A1:U40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="J2" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="I3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="53">
+        <v>860246</v>
+      </c>
+      <c r="K3" s="54">
+        <f>+J3/J15</f>
+        <v>0.87508748372395828</v>
+      </c>
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="I4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="16">
+        <v>1250269</v>
+      </c>
+      <c r="K4" s="52">
+        <f>+J4/J16</f>
+        <v>0.47693977355957029</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <f>+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(S2,+LEN(D2)-2)),"")</f>
+        <v>36864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="61"/>
+      <c r="K12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" s="39"/>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="str">
+        <f t="shared" ref="A13:A19" si="0">IF(A2&lt;&gt;"",+A2,"")</f>
+        <v>nvs</v>
+      </c>
+      <c r="B13" s="11">
+        <f t="shared" ref="B13:C19" si="1">+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(D2,+LEN(D2)-2)),"")</f>
+        <v>36864</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="1"/>
+        <v>20480</v>
+      </c>
+      <c r="D13" s="23">
+        <f>+IF($A13&lt;&gt;"",+B13+C13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="38">
+        <f>+IF($E13&lt;&gt;"",+B13,"")</f>
+        <v>36864</v>
+      </c>
+      <c r="I13" s="28">
+        <f>+IF($E13&lt;&gt;"",+C13,"")/1024</f>
+        <v>20</v>
+      </c>
+      <c r="J13" s="28">
+        <f>+I13*1024</f>
+        <v>20480</v>
+      </c>
+      <c r="K13" s="41">
+        <f>+IF($E13&lt;&gt;"",+H13+J13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="L13" s="42">
+        <f t="shared" ref="L13:L19" si="2">+J13/1024</f>
+        <v>20</v>
+      </c>
+      <c r="M13" s="42">
+        <f t="shared" ref="M13:M19" si="3">+IF($E13&lt;&gt;"",($K$20-K13)/1024,"")</f>
+        <v>4040</v>
+      </c>
+      <c r="O13" s="18"/>
+      <c r="P13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>otadata</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="1"/>
+        <v>57344</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="D14" s="24">
+        <f t="shared" ref="D14:D19" si="4">+IF($A14&lt;&gt;"",+B14+C14,"")</f>
+        <v>65536</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="43">
+        <f t="shared" ref="H14:H19" si="5">+IF($E14&lt;&gt;"",+K13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="I14" s="26">
+        <f>+IF($E14&lt;&gt;"",+C14,"")/1024</f>
+        <v>8</v>
+      </c>
+      <c r="J14" s="26">
+        <f>+I14*1024</f>
+        <v>8192</v>
+      </c>
+      <c r="K14" s="44">
+        <f t="shared" ref="K14:K19" si="6">+IF($E14&lt;&gt;"",+H14+J14,"")</f>
+        <v>65536</v>
+      </c>
+      <c r="L14" s="42">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M14" s="42">
+        <f t="shared" si="3"/>
+        <v>4032</v>
+      </c>
+      <c r="O14" s="45"/>
+      <c r="P14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>app0</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>917504</v>
+      </c>
+      <c r="D15" s="24">
+        <f t="shared" si="4"/>
+        <v>983040</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="43">
+        <f t="shared" si="5"/>
+        <v>65536</v>
+      </c>
+      <c r="I15" s="46">
+        <f>15*64</f>
+        <v>960</v>
+      </c>
+      <c r="J15" s="46">
+        <f>+I15*1024</f>
+        <v>983040</v>
+      </c>
+      <c r="K15" s="44">
+        <f t="shared" si="6"/>
+        <v>1048576</v>
+      </c>
+      <c r="L15" s="42">
+        <f t="shared" si="2"/>
+        <v>960</v>
+      </c>
+      <c r="M15" s="42">
+        <f t="shared" si="3"/>
+        <v>3072</v>
+      </c>
+      <c r="O15" s="47"/>
+      <c r="P15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>app1</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="1"/>
+        <v>983040</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="1"/>
+        <v>3160064</v>
+      </c>
+      <c r="D16" s="24">
+        <f t="shared" si="4"/>
+        <v>4143104</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="43">
+        <f t="shared" si="5"/>
+        <v>1048576</v>
+      </c>
+      <c r="I16" s="46">
+        <f>40*64</f>
+        <v>2560</v>
+      </c>
+      <c r="J16" s="46">
+        <f>+I16*1024</f>
+        <v>2621440</v>
+      </c>
+      <c r="K16" s="44">
+        <f t="shared" si="6"/>
+        <v>3670016</v>
+      </c>
+      <c r="L16" s="42">
+        <f t="shared" si="2"/>
+        <v>2560</v>
+      </c>
+      <c r="M16" s="42">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>spiffs</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="1"/>
+        <v>4143104</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>51200</v>
+      </c>
+      <c r="D17" s="24">
+        <f t="shared" si="4"/>
+        <v>4194304</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="43">
+        <f t="shared" si="5"/>
+        <v>3670016</v>
+      </c>
+      <c r="I17" s="46">
+        <f>8*64</f>
+        <v>512</v>
+      </c>
+      <c r="J17" s="46">
+        <f>+I17*1024</f>
+        <v>524288</v>
+      </c>
+      <c r="K17" s="44">
+        <f t="shared" si="6"/>
+        <v>4194304</v>
+      </c>
+      <c r="L17" s="42">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+      <c r="M17" s="42">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D18" s="24" t="str">
+        <f>+IF($A18&lt;&gt;"",+B18+C18,"")</f>
+        <v/>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="43" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="44" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="L18" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="42" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B19" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D19" s="25" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="48" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="50" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="L19" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="42" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="R19" s="19"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="51"/>
+      <c r="K20" s="1">
+        <f>4*1024*1024</f>
+        <v>4194304</v>
+      </c>
+      <c r="L20" s="19">
+        <f>SUM(L13:L19)+H13/1024</f>
+        <v>4096</v>
+      </c>
+      <c r="R20" s="19"/>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="str">
+        <f t="shared" ref="A23:A29" si="7">+IF(E13&lt;&gt;"",E13,"")</f>
+        <v>nvs</v>
+      </c>
+      <c r="B23" s="11" t="str">
+        <f t="shared" ref="B23:C29" si="8">+IF($A23&lt;&gt;"",F13,"")</f>
+        <v>data</v>
+      </c>
+      <c r="C23" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>nvs</v>
+      </c>
+      <c r="D23" s="11" t="str">
+        <f t="shared" ref="D23:D29" si="9">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(H13,6)),"")</f>
+        <v>0x009000</v>
+      </c>
+      <c r="E23" s="11" t="str">
+        <f t="shared" ref="E23:E29" si="10">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(J13,6)),"")</f>
+        <v>0x005000</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="H23">
+        <f>+IF($E23&lt;&gt;"",HEX2DEC(RIGHT(E23,+LEN(E23)-2)),"")</f>
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>otadata</v>
+      </c>
+      <c r="B24" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>data</v>
+      </c>
+      <c r="C24" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>ota</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x00E000</v>
+      </c>
+      <c r="E24" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x002000</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="H24">
+        <f t="shared" ref="H24:H27" si="11">+IF($E24&lt;&gt;"",HEX2DEC(RIGHT(E24,+LEN(E24)-2)),"")</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>Loader</v>
+      </c>
+      <c r="B25" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>app</v>
+      </c>
+      <c r="C25" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>ota_0</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x010000</v>
+      </c>
+      <c r="E25" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x0F0000</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="H25">
+        <f t="shared" si="11"/>
+        <v>983040</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>app</v>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>app</v>
+      </c>
+      <c r="C26" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>ota_1</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x100000</v>
+      </c>
+      <c r="E26" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x280000</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="H26">
+        <f t="shared" si="11"/>
+        <v>2621440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>spiffs</v>
+      </c>
+      <c r="B27" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>data</v>
+      </c>
+      <c r="C27" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>spiffs</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x380000</v>
+      </c>
+      <c r="E27" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x080000</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="H27">
+        <f t="shared" si="11"/>
+        <v>524288</v>
+      </c>
+      <c r="N27">
+        <f>0.875*1024</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B28" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E28" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="I28">
+        <v>4096</v>
+      </c>
+      <c r="N28">
+        <f>900*1024</f>
+        <v>921600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B29" s="16" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="C29" s="16" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="D29" s="16" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E29" s="16" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="I29">
+        <f>36+I13+I14+I16+I17</f>
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>+I28-I29</f>
+        <v>960</v>
+      </c>
+      <c r="K30">
+        <f>+I30</f>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f>+INT(K30/64)*64</f>
+        <v>960</v>
+      </c>
+      <c r="L31">
+        <f>+K31+64</f>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E32" t="e">
+        <f>+D25+E25</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>+CONCATENATE(A22,", ",B22,", ",C22,", ",D22,", ",E22,", ",F22)</f>
+        <v># Name, Type, SubType, Offset, Size, Flags</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" ref="A34:A40" si="12">+CONCATENATE(A23,", ",B23,", ",C23,", ",D23,", ",E23,", ",F23)</f>
+        <v xml:space="preserve">nvs, data, nvs, 0x009000, 0x005000, </v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">otadata, data, ota, 0x00E000, 0x002000, </v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">Loader, app, ota_0, 0x010000, 0x0F0000, </v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">app, app, ota_1, 0x100000, 0x280000, </v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">spiffs, data, spiffs, 0x380000, 0x080000, </v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, , , , , </v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, , , , , </v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B43E6B0-5B54-428C-9D5E-D5F8106930A6}">
+  <dimension ref="A1:U40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="J2" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="I3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="53">
+        <v>860246</v>
+      </c>
+      <c r="K3" s="54">
+        <f>+J3/J15</f>
+        <v>0.48615971317997686</v>
+      </c>
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="I4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="16">
+        <v>1288481</v>
+      </c>
+      <c r="K4" s="52">
+        <f>+J4/J16</f>
+        <v>0.72817258481626157</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <f>+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(S2,+LEN(D2)-2)),"")</f>
+        <v>36864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="61"/>
+      <c r="K12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" s="39"/>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="str">
+        <f t="shared" ref="A13:A19" si="0">IF(A2&lt;&gt;"",+A2,"")</f>
+        <v>nvs</v>
+      </c>
+      <c r="B13" s="11">
+        <f t="shared" ref="B13:C19" si="1">+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(D2,+LEN(D2)-2)),"")</f>
+        <v>36864</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="1"/>
+        <v>20480</v>
+      </c>
+      <c r="D13" s="23">
+        <f>+IF($A13&lt;&gt;"",+B13+C13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="38">
+        <f>+IF($E13&lt;&gt;"",+B13,"")</f>
+        <v>36864</v>
+      </c>
+      <c r="I13" s="28">
+        <f>+IF($E13&lt;&gt;"",+C13,"")/1024</f>
+        <v>20</v>
+      </c>
+      <c r="J13" s="28">
+        <f>+I13*1024</f>
+        <v>20480</v>
+      </c>
+      <c r="K13" s="41">
+        <f>+IF($E13&lt;&gt;"",+H13+J13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="L13" s="42">
+        <f t="shared" ref="L13:L19" si="2">+J13/1024</f>
+        <v>20</v>
+      </c>
+      <c r="M13" s="42">
+        <f t="shared" ref="M13:M19" si="3">+IF($E13&lt;&gt;"",($K$20-K13)/1024,"")</f>
+        <v>4040</v>
+      </c>
+      <c r="O13" s="18"/>
+      <c r="P13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>otadata</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="1"/>
+        <v>57344</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="D14" s="24">
+        <f t="shared" ref="D14:D19" si="4">+IF($A14&lt;&gt;"",+B14+C14,"")</f>
+        <v>65536</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="43">
+        <f t="shared" ref="H14:H19" si="5">+IF($E14&lt;&gt;"",+K13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="I14" s="26">
+        <f>+IF($E14&lt;&gt;"",+C14,"")/1024</f>
+        <v>8</v>
+      </c>
+      <c r="J14" s="26">
+        <f>+I14*1024</f>
+        <v>8192</v>
+      </c>
+      <c r="K14" s="44">
+        <f t="shared" ref="K14:K19" si="6">+IF($E14&lt;&gt;"",+H14+J14,"")</f>
+        <v>65536</v>
+      </c>
+      <c r="L14" s="42">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M14" s="42">
+        <f t="shared" si="3"/>
+        <v>4032</v>
+      </c>
+      <c r="O14" s="45"/>
+      <c r="P14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>app0</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>917504</v>
+      </c>
+      <c r="D15" s="24">
+        <f t="shared" si="4"/>
+        <v>983040</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="43">
+        <f t="shared" si="5"/>
+        <v>65536</v>
+      </c>
+      <c r="I15" s="46">
+        <f>27*64</f>
+        <v>1728</v>
+      </c>
+      <c r="J15" s="46">
+        <f>+I15*1024</f>
+        <v>1769472</v>
+      </c>
+      <c r="K15" s="44">
+        <f t="shared" si="6"/>
+        <v>1835008</v>
+      </c>
+      <c r="L15" s="42">
+        <f t="shared" si="2"/>
+        <v>1728</v>
+      </c>
+      <c r="M15" s="42">
+        <f t="shared" si="3"/>
+        <v>2304</v>
+      </c>
+      <c r="O15" s="47"/>
+      <c r="P15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>app1</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="1"/>
+        <v>983040</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="1"/>
+        <v>3160064</v>
+      </c>
+      <c r="D16" s="24">
+        <f t="shared" si="4"/>
+        <v>4143104</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="43">
+        <f t="shared" si="5"/>
+        <v>1835008</v>
+      </c>
+      <c r="I16" s="46">
+        <f>27*64</f>
+        <v>1728</v>
+      </c>
+      <c r="J16" s="46">
+        <f>+I16*1024</f>
+        <v>1769472</v>
+      </c>
+      <c r="K16" s="44">
+        <f t="shared" si="6"/>
+        <v>3604480</v>
+      </c>
+      <c r="L16" s="42">
+        <f t="shared" si="2"/>
+        <v>1728</v>
+      </c>
+      <c r="M16" s="42">
+        <f t="shared" si="3"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>spiffs</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="1"/>
+        <v>4143104</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="1"/>
+        <v>51200</v>
+      </c>
+      <c r="D17" s="24">
+        <f t="shared" si="4"/>
+        <v>4194304</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="43">
+        <f t="shared" si="5"/>
+        <v>3604480</v>
+      </c>
+      <c r="I17" s="46">
+        <f>8*64</f>
+        <v>512</v>
+      </c>
+      <c r="J17" s="46">
+        <f>+I17*1024</f>
+        <v>524288</v>
+      </c>
+      <c r="K17" s="44">
+        <f t="shared" si="6"/>
+        <v>4128768</v>
+      </c>
+      <c r="L17" s="42">
+        <f t="shared" si="2"/>
+        <v>512</v>
+      </c>
+      <c r="M17" s="42">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D18" s="24" t="str">
+        <f>+IF($A18&lt;&gt;"",+B18+C18,"")</f>
+        <v/>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="43" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="44" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="L18" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="42" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B19" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D19" s="25" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="48" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="50" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="L19" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="42" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="R19" s="19"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="51"/>
+      <c r="K20" s="1">
+        <f>4*1024*1024</f>
+        <v>4194304</v>
+      </c>
+      <c r="L20" s="19">
+        <f>SUM(L13:L19)+H13/1024</f>
+        <v>4032</v>
+      </c>
+      <c r="R20" s="19"/>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="str">
+        <f t="shared" ref="A23:A29" si="7">+IF(E13&lt;&gt;"",E13,"")</f>
+        <v>nvs</v>
+      </c>
+      <c r="B23" s="11" t="str">
+        <f t="shared" ref="B23:C29" si="8">+IF($A23&lt;&gt;"",F13,"")</f>
+        <v>data</v>
+      </c>
+      <c r="C23" s="11" t="str">
+        <f t="shared" si="8"/>
+        <v>nvs</v>
+      </c>
+      <c r="D23" s="11" t="str">
+        <f t="shared" ref="D23:D29" si="9">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(H13,6)),"")</f>
+        <v>0x009000</v>
+      </c>
+      <c r="E23" s="11" t="str">
+        <f t="shared" ref="E23:E29" si="10">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(J13,6)),"")</f>
+        <v>0x005000</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="H23">
+        <f>+IF($E23&lt;&gt;"",HEX2DEC(RIGHT(E23,+LEN(E23)-2)),"")</f>
+        <v>20480</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>otadata</v>
+      </c>
+      <c r="B24" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>data</v>
+      </c>
+      <c r="C24" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>ota</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x00E000</v>
+      </c>
+      <c r="E24" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x002000</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="H24">
+        <f t="shared" ref="H24:H27" si="11">+IF($E24&lt;&gt;"",HEX2DEC(RIGHT(E24,+LEN(E24)-2)),"")</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>Loader</v>
+      </c>
+      <c r="B25" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>app</v>
+      </c>
+      <c r="C25" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>ota_0</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x010000</v>
+      </c>
+      <c r="E25" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x1B0000</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="H25">
+        <f t="shared" si="11"/>
+        <v>1769472</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>app</v>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>app</v>
+      </c>
+      <c r="C26" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>ota_1</v>
+      </c>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x1C0000</v>
+      </c>
+      <c r="E26" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x1B0000</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="H26">
+        <f t="shared" si="11"/>
+        <v>1769472</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v>spiffs</v>
+      </c>
+      <c r="B27" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>data</v>
+      </c>
+      <c r="C27" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>spiffs</v>
+      </c>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v>0x370000</v>
+      </c>
+      <c r="E27" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v>0x080000</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="H27">
+        <f t="shared" si="11"/>
+        <v>524288</v>
+      </c>
+      <c r="N27">
+        <f>0.875*1024</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B28" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="D28" s="6" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E28" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="I28">
+        <v>4096</v>
+      </c>
+      <c r="N28">
+        <f>900*1024</f>
+        <v>921600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B29" s="16" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="C29" s="16" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="D29" s="16" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E29" s="16" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="I29">
+        <f>36+I13+I14+I16+I17</f>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>+I28-I29</f>
+        <v>1792</v>
+      </c>
+      <c r="K30">
+        <f>+I30</f>
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f>+INT(K30/64)*64</f>
+        <v>1792</v>
+      </c>
+      <c r="L31">
+        <f>+K31+64</f>
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E32" t="e">
+        <f>+D25+E25</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>+CONCATENATE(A22,", ",B22,", ",C22,", ",D22,", ",E22,", ",F22)</f>
+        <v># Name, Type, SubType, Offset, Size, Flags</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" ref="A34:A40" si="12">+CONCATENATE(A23,", ",B23,", ",C23,", ",D23,", ",E23,", ",F23)</f>
+        <v xml:space="preserve">nvs, data, nvs, 0x009000, 0x005000, </v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">otadata, data, ota, 0x00E000, 0x002000, </v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">Loader, app, ota_0, 0x010000, 0x1B0000, </v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">app, app, ota_1, 0x1C0000, 0x1B0000, </v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">spiffs, data, spiffs, 0x370000, 0x080000, </v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, , , , , </v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, , , , , </v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras en la asociacion, activacion BLE y nombre WiFi
Cambios:
-Mejoras en la activacion de la plataforma
-BLE
-Nombre dispositivo en WiFi igual al nombre de servicio (SID)
-Info incluye MAC y nombre WiFi
-Deprecado nombre dispositivo en config.json y ID_MQTT en MQTTConfig.json
-Añadida particion para cores
-Reordenados los dispositivos en platformio.ini
-Primera entrega desde reinstalacion PC
</commit_message>
<xml_diff>
--- a/.mio/Particiones_ESP32_v2.xlsx
+++ b/.mio/Particiones_ESP32_v2.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlopezt\Documents\PlatformIO\Projects\Actuador-ESP32\.mio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e46e0175a720d0fc/Documents/PlatformIO/Projects/Actuador-ESP32/.mio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6836DE-4D01-4628-B4F2-5955A07092EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{57EECD15-8379-4BA6-911C-C2850916100C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30593A60-ECB8-49E2-8C77-D8B0696B551B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{A52EA33D-BD66-4045-9139-39A15A538EC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{A52EA33D-BD66-4045-9139-39A15A538EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="esquema con cargador" sheetId="2" r:id="rId1"/>
     <sheet name="esquema con cargador y SPIFFS" sheetId="3" r:id="rId2"/>
     <sheet name="esquema simetrico y SPIFFS" sheetId="4" r:id="rId3"/>
+    <sheet name="simetrico y SPIFFS (coredump)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="80">
   <si>
     <t>Flags</t>
   </si>
@@ -254,6 +255,27 @@
   </si>
   <si>
     <t>Ocupación</t>
+  </si>
+  <si>
+    <t>coredump</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> coredump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        64K</t>
+  </si>
+  <si>
+    <t>Con BT</t>
+  </si>
+  <si>
+    <t>Sin BT</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>kB</t>
   </si>
 </sst>
 </file>
@@ -263,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,6 +313,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF404040"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -798,13 +826,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -826,20 +853,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -859,6 +882,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,7 +1219,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951BFC8B-84AC-47C7-AF9F-2926E2701612}">
-  <dimension ref="A1:T44"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
@@ -1206,22 +1232,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="O1" t="s">
@@ -1244,22 +1270,22 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="11"/>
       <c r="O2" t="s">
         <v>5</v>
       </c>
@@ -1277,22 +1303,22 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="13"/>
       <c r="O3" t="s">
         <v>9</v>
       </c>
@@ -1310,22 +1336,22 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="13"/>
       <c r="O4" t="s">
         <v>13</v>
       </c>
@@ -1343,22 +1369,22 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
       <c r="O5" t="s">
         <v>23</v>
       </c>
@@ -1376,22 +1402,22 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="O6" t="s">
         <v>18</v>
       </c>
@@ -1409,62 +1435,54 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60" t="s">
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="62"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="33" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
@@ -1482,673 +1500,567 @@
       <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="N12" s="39"/>
+      <c r="N12" s="35"/>
       <c r="O12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="str">
+      <c r="A13" s="9" t="str">
         <f t="shared" ref="A13:A19" si="0">IF(A2&lt;&gt;"",+A2,"")</f>
         <v>nvs</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <f t="shared" ref="B13:C19" si="1">+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(D2,+LEN(D2)-2)),"")</f>
         <v>36864</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <f t="shared" si="1"/>
         <v>20480</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f>+IF($A13&lt;&gt;"",+B13+C13,"")</f>
         <v>57344</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="34">
         <f>+IF($E13&lt;&gt;"",+B13,"")</f>
         <v>36864</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="26">
         <f>+IF($E13&lt;&gt;"",+C13,"")</f>
         <v>20480</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="11">
         <f>+IF($E13&lt;&gt;"",+H13+I13,"")</f>
         <v>57344</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="18">
         <f>+I13/1024/1024</f>
         <v>1.953125E-2</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="18">
         <f>+IF($E13&lt;&gt;"",($J$20-J13)/1024/1024,"")</f>
         <v>3.9453125</v>
       </c>
-      <c r="N13" s="18"/>
+      <c r="N13" s="17"/>
       <c r="O13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="str">
+      <c r="A14" s="12" t="str">
         <f t="shared" si="0"/>
         <v>otadata</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f t="shared" si="1"/>
         <v>57344</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <f t="shared" ref="D14:D19" si="2">+IF($A14&lt;&gt;"",+B14+C14,"")</f>
         <v>65536</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" ref="H14:H19" si="3">+IF($E14&lt;&gt;"",+J13,"")</f>
         <v>57344</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>+IF($E14&lt;&gt;"",+C14,"")</f>
         <v>8192</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <f t="shared" ref="J14:J19" si="4">+IF($E14&lt;&gt;"",+H14+I14,"")</f>
         <v>65536</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="18">
         <f t="shared" ref="K14:K19" si="5">+I14/1024/1024</f>
         <v>7.8125E-3</v>
       </c>
-      <c r="L14" s="19">
+      <c r="L14" s="18">
         <f t="shared" ref="L14:L19" si="6">+IF($E14&lt;&gt;"",($J$20-J14)/1024/1024,"")</f>
         <v>3.9375</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="str">
+      <c r="A15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>app0</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <f t="shared" si="1"/>
         <v>1310720</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <f t="shared" si="2"/>
         <v>1376256</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="3"/>
         <v>65536</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <f>1.5*1024*1024</f>
         <v>1572864</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <f t="shared" si="4"/>
         <v>1638400</v>
       </c>
-      <c r="K15" s="19">
+      <c r="K15" s="18">
         <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
-      <c r="L15" s="19">
+      <c r="L15" s="18">
         <f t="shared" si="6"/>
         <v>2.4375</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="12" t="str">
         <f t="shared" si="0"/>
         <v>app1</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f t="shared" si="1"/>
         <v>1376256</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <f t="shared" si="1"/>
         <v>1310720</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <f t="shared" si="2"/>
         <v>2686976</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="3"/>
         <v>1638400</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <f>1.5*1024*1024</f>
         <v>1572864</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f t="shared" si="4"/>
         <v>3211264</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="18">
         <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="18">
         <f t="shared" si="6"/>
         <v>0.9375</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="str">
+      <c r="A17" s="12" t="str">
         <f t="shared" si="0"/>
         <v>spiffs</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f t="shared" si="1"/>
         <v>2686976</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <f t="shared" si="1"/>
         <v>1507328</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <f t="shared" si="2"/>
         <v>4194304</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f t="shared" si="3"/>
         <v>3211264</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <f>(0.9375)*1024*1024</f>
         <v>983040</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <f t="shared" si="4"/>
         <v>4194304</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <f t="shared" si="5"/>
         <v>0.9375</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="18">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="str">
+      <c r="A18" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B18" s="6" t="str">
+      <c r="B18" s="5" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="5" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D18" s="24" t="str">
+      <c r="D18" s="23" t="str">
         <f>+IF($A18&lt;&gt;"",+B18+C18,"")</f>
         <v/>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="6" t="str">
+      <c r="E18" s="31"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="14" t="str">
+      <c r="I18" s="5"/>
+      <c r="J18" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L18" s="19" t="str">
+      <c r="L18" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="str">
+      <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B19" s="16" t="str">
+      <c r="B19" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D19" s="25" t="str">
+      <c r="D19" s="24" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16" t="str">
+      <c r="E19" s="32"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17" t="str">
+      <c r="I19" s="15"/>
+      <c r="J19" s="16" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L19" s="19" t="str">
+      <c r="L19" s="18" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="Q19" s="19"/>
+      <c r="Q19" s="18"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J20" s="1">
         <f>4*1024*1024</f>
         <v>4194304</v>
       </c>
-      <c r="K20" s="19">
+      <c r="K20" s="18">
         <f>SUM(K13:K19)+H13/1024/1024</f>
         <v>4</v>
       </c>
-      <c r="Q20" s="19"/>
+      <c r="Q20" s="18"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="str">
+      <c r="A23" s="9" t="str">
         <f t="shared" ref="A23:A29" si="7">+IF(E13&lt;&gt;"",E13,"")</f>
         <v>nvs</v>
       </c>
-      <c r="B23" s="11" t="str">
+      <c r="B23" s="10" t="str">
         <f t="shared" ref="B23:C29" si="8">+IF($A23&lt;&gt;"",F13,"")</f>
         <v>data</v>
       </c>
-      <c r="C23" s="11" t="str">
+      <c r="C23" s="10" t="str">
         <f t="shared" si="8"/>
         <v>nvs</v>
       </c>
-      <c r="D23" s="11" t="str">
+      <c r="D23" s="10" t="str">
         <f t="shared" ref="D23:E29" si="9">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(H13,6)),"")</f>
         <v>0x009000</v>
       </c>
-      <c r="E23" s="11" t="str">
+      <c r="E23" s="10" t="str">
         <f t="shared" si="9"/>
         <v>0x005000</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="str">
+      <c r="A24" s="12" t="str">
         <f t="shared" si="7"/>
         <v>otadata</v>
       </c>
-      <c r="B24" s="6" t="str">
+      <c r="B24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>data</v>
       </c>
-      <c r="C24" s="6" t="str">
+      <c r="C24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota</v>
       </c>
-      <c r="D24" s="6" t="str">
+      <c r="D24" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x00E000</v>
       </c>
-      <c r="E24" s="6" t="str">
+      <c r="E24" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x002000</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
+      <c r="A25" s="12" t="str">
         <f t="shared" si="7"/>
         <v>Loader</v>
       </c>
-      <c r="B25" s="6" t="str">
+      <c r="B25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>app</v>
       </c>
-      <c r="C25" s="6" t="str">
+      <c r="C25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota_0</v>
       </c>
-      <c r="D25" s="6" t="str">
+      <c r="D25" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x010000</v>
       </c>
-      <c r="E25" s="6" t="str">
+      <c r="E25" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x180000</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
+      <c r="A26" s="12" t="str">
         <f t="shared" si="7"/>
         <v>app</v>
       </c>
-      <c r="B26" s="6" t="str">
+      <c r="B26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>app</v>
       </c>
-      <c r="C26" s="6" t="str">
+      <c r="C26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota_1</v>
       </c>
-      <c r="D26" s="6" t="str">
+      <c r="D26" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x190000</v>
       </c>
-      <c r="E26" s="6" t="str">
+      <c r="E26" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x180000</v>
       </c>
-      <c r="F26" s="14"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
+      <c r="A27" s="12" t="str">
         <f t="shared" si="7"/>
         <v>spiffs</v>
       </c>
-      <c r="B27" s="6" t="str">
+      <c r="B27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>data</v>
       </c>
-      <c r="C27" s="6" t="str">
+      <c r="C27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>spiffs</v>
       </c>
-      <c r="D27" s="6" t="str">
+      <c r="D27" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x310000</v>
       </c>
-      <c r="E27" s="6" t="str">
+      <c r="E27" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x0F0000</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
+      <c r="A28" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="B28" s="6" t="str">
+      <c r="B28" s="5" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="C28" s="6" t="str">
+      <c r="C28" s="5" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D28" s="6" t="str">
+      <c r="D28" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E28" s="6" t="str">
+      <c r="E28" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="F28" s="14"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="str">
+      <c r="A29" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="B29" s="16" t="str">
+      <c r="B29" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D29" s="16" t="str">
+      <c r="D29" s="15" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E29" s="16" t="str">
+      <c r="E29" s="15" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="F29" s="17"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F29" s="16"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>+CONCATENATE(A22,", ",B22,", ",C22,", ",D22,", ",E22,", ",F22)</f>
         <v># Name, Type, SubType, Offset, Size, Flags</v>
       </c>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" ref="A34:A40" si="10">+CONCATENATE(A23,", ",B23,", ",C23,", ",D23,", ",E23,", ",F23)</f>
         <v xml:space="preserve">nvs, data, nvs, 0x009000, 0x005000, </v>
       </c>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">otadata, data, ota, 0x00E000, 0x002000, </v>
       </c>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">Loader, app, ota_0, 0x010000, 0x180000, </v>
       </c>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">app, app, ota_1, 0x190000, 0x180000, </v>
       </c>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">spiffs, data, spiffs, 0x310000, 0x0F0000, </v>
       </c>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">, , , , , </v>
       </c>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="10"/>
         <v xml:space="preserve">, , , , , </v>
       </c>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2176,22 +2088,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="P1" t="s">
@@ -2214,26 +2126,26 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="J2" s="55" t="s">
+      <c r="F2" s="11"/>
+      <c r="J2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="51" t="s">
         <v>72</v>
       </c>
       <c r="P2" t="s">
@@ -2256,29 +2168,29 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="I3" s="10" t="s">
+      <c r="F3" s="13"/>
+      <c r="I3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="53">
+      <c r="J3" s="48">
         <v>860246</v>
       </c>
-      <c r="K3" s="54">
+      <c r="K3" s="49">
         <f>+J3/J15</f>
         <v>0.87508748372395828</v>
       </c>
@@ -2302,29 +2214,29 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="I4" s="15" t="s">
+      <c r="F4" s="13"/>
+      <c r="I4" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>1250269</v>
       </c>
-      <c r="K4" s="52">
+      <c r="K4" s="47">
         <f>+J4/J16</f>
         <v>0.47693977355957029</v>
       </c>
@@ -2348,22 +2260,22 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
       <c r="P5" t="s">
         <v>14</v>
       </c>
@@ -2384,22 +2296,22 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="P6" t="s">
         <v>18</v>
       </c>
@@ -2417,20 +2329,20 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S9">
@@ -2440,47 +2352,47 @@
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60" t="s">
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="33" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="61"/>
+      <c r="J12" s="57"/>
       <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
@@ -2490,522 +2402,522 @@
       <c r="M12" t="s">
         <v>67</v>
       </c>
-      <c r="O12" s="39"/>
+      <c r="O12" s="35"/>
       <c r="P12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="str">
+      <c r="A13" s="9" t="str">
         <f t="shared" ref="A13:A19" si="0">IF(A2&lt;&gt;"",+A2,"")</f>
         <v>nvs</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <f t="shared" ref="B13:C19" si="1">+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(D2,+LEN(D2)-2)),"")</f>
         <v>36864</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <f t="shared" si="1"/>
         <v>20480</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f>+IF($A13&lt;&gt;"",+B13+C13,"")</f>
         <v>57344</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="34">
         <f>+IF($E13&lt;&gt;"",+B13,"")</f>
         <v>36864</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="26">
         <f>+IF($E13&lt;&gt;"",+C13,"")/1024</f>
         <v>20</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="26">
         <f>+I13*1024</f>
         <v>20480</v>
       </c>
-      <c r="K13" s="41">
+      <c r="K13" s="36">
         <f>+IF($E13&lt;&gt;"",+H13+J13,"")</f>
         <v>57344</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="37">
         <f t="shared" ref="L13:L19" si="2">+J13/1024</f>
         <v>20</v>
       </c>
-      <c r="M13" s="42">
+      <c r="M13" s="37">
         <f t="shared" ref="M13:M19" si="3">+IF($E13&lt;&gt;"",($K$20-K13)/1024,"")</f>
         <v>4040</v>
       </c>
-      <c r="O13" s="18"/>
+      <c r="O13" s="17"/>
       <c r="P13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="str">
+      <c r="A14" s="12" t="str">
         <f t="shared" si="0"/>
         <v>otadata</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f t="shared" si="1"/>
         <v>57344</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <f t="shared" ref="D14:D19" si="4">+IF($A14&lt;&gt;"",+B14+C14,"")</f>
         <v>65536</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="38">
         <f t="shared" ref="H14:H19" si="5">+IF($E14&lt;&gt;"",+K13,"")</f>
         <v>57344</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>+IF($E14&lt;&gt;"",+C14,"")/1024</f>
         <v>8</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="25">
         <f>+I14*1024</f>
         <v>8192</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="39">
         <f t="shared" ref="K14:K19" si="6">+IF($E14&lt;&gt;"",+H14+J14,"")</f>
         <v>65536</v>
       </c>
-      <c r="L14" s="42">
+      <c r="L14" s="37">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="M14" s="42">
+      <c r="M14" s="37">
         <f t="shared" si="3"/>
         <v>4032</v>
       </c>
-      <c r="O14" s="45"/>
+      <c r="O14" s="40"/>
       <c r="P14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="str">
+      <c r="A15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>app0</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <f t="shared" si="1"/>
         <v>917504</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <f t="shared" si="4"/>
         <v>983040</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H15" s="38">
         <f t="shared" si="5"/>
         <v>65536</v>
       </c>
-      <c r="I15" s="46">
+      <c r="I15" s="41">
         <f>15*64</f>
         <v>960</v>
       </c>
-      <c r="J15" s="46">
+      <c r="J15" s="41">
         <f>+I15*1024</f>
         <v>983040</v>
       </c>
-      <c r="K15" s="44">
+      <c r="K15" s="39">
         <f t="shared" si="6"/>
         <v>1048576</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="37">
         <f t="shared" si="2"/>
         <v>960</v>
       </c>
-      <c r="M15" s="42">
+      <c r="M15" s="37">
         <f t="shared" si="3"/>
         <v>3072</v>
       </c>
-      <c r="O15" s="47"/>
+      <c r="O15" s="42"/>
       <c r="P15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="12" t="str">
         <f t="shared" si="0"/>
         <v>app1</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f t="shared" si="1"/>
         <v>983040</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <f t="shared" si="1"/>
         <v>3160064</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <f t="shared" si="4"/>
         <v>4143104</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="43">
+      <c r="H16" s="38">
         <f t="shared" si="5"/>
         <v>1048576</v>
       </c>
-      <c r="I16" s="46">
+      <c r="I16" s="41">
         <f>40*64</f>
         <v>2560</v>
       </c>
-      <c r="J16" s="46">
+      <c r="J16" s="41">
         <f>+I16*1024</f>
         <v>2621440</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="39">
         <f t="shared" si="6"/>
         <v>3670016</v>
       </c>
-      <c r="L16" s="42">
+      <c r="L16" s="37">
         <f t="shared" si="2"/>
         <v>2560</v>
       </c>
-      <c r="M16" s="42">
+      <c r="M16" s="37">
         <f t="shared" si="3"/>
         <v>512</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="str">
+      <c r="A17" s="12" t="str">
         <f t="shared" si="0"/>
         <v>spiffs</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f t="shared" si="1"/>
         <v>4143104</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <f t="shared" si="1"/>
         <v>51200</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <f t="shared" si="4"/>
         <v>4194304</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="43">
+      <c r="H17" s="38">
         <f t="shared" si="5"/>
         <v>3670016</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="41">
         <f>8*64</f>
         <v>512</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="41">
         <f>+I17*1024</f>
         <v>524288</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="39">
         <f t="shared" si="6"/>
         <v>4194304</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L17" s="37">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="37">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="str">
+      <c r="A18" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B18" s="6" t="str">
+      <c r="B18" s="5" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="5" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D18" s="24" t="str">
+      <c r="D18" s="23" t="str">
         <f>+IF($A18&lt;&gt;"",+B18+C18,"")</f>
         <v/>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="43" t="str">
+      <c r="E18" s="31"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="38" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="44" t="str">
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="39" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" s="42" t="str">
+      <c r="M18" s="37" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="str">
+      <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B19" s="16" t="str">
+      <c r="B19" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D19" s="25" t="str">
+      <c r="D19" s="24" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="48" t="str">
+      <c r="E19" s="32"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="43" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50" t="str">
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="L19" s="42">
+      <c r="L19" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" s="42" t="str">
+      <c r="M19" s="37" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="R19" s="19"/>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="51"/>
+      <c r="C20" s="46"/>
       <c r="K20" s="1">
         <f>4*1024*1024</f>
         <v>4194304</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="18">
         <f>SUM(L13:L19)+H13/1024</f>
         <v>4096</v>
       </c>
-      <c r="R20" s="19"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L21" s="19"/>
+      <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="str">
+      <c r="A23" s="9" t="str">
         <f t="shared" ref="A23:A29" si="7">+IF(E13&lt;&gt;"",E13,"")</f>
         <v>nvs</v>
       </c>
-      <c r="B23" s="11" t="str">
+      <c r="B23" s="10" t="str">
         <f t="shared" ref="B23:C29" si="8">+IF($A23&lt;&gt;"",F13,"")</f>
         <v>data</v>
       </c>
-      <c r="C23" s="11" t="str">
+      <c r="C23" s="10" t="str">
         <f t="shared" si="8"/>
         <v>nvs</v>
       </c>
-      <c r="D23" s="11" t="str">
+      <c r="D23" s="10" t="str">
         <f t="shared" ref="D23:D29" si="9">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(H13,6)),"")</f>
         <v>0x009000</v>
       </c>
-      <c r="E23" s="11" t="str">
+      <c r="E23" s="10" t="str">
         <f t="shared" ref="E23:E29" si="10">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(J13,6)),"")</f>
         <v>0x005000</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="11"/>
       <c r="H23">
         <f>+IF($E23&lt;&gt;"",HEX2DEC(RIGHT(E23,+LEN(E23)-2)),"")</f>
         <v>20480</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="str">
+      <c r="A24" s="12" t="str">
         <f t="shared" si="7"/>
         <v>otadata</v>
       </c>
-      <c r="B24" s="6" t="str">
+      <c r="B24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>data</v>
       </c>
-      <c r="C24" s="6" t="str">
+      <c r="C24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota</v>
       </c>
-      <c r="D24" s="6" t="str">
+      <c r="D24" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x00E000</v>
       </c>
-      <c r="E24" s="6" t="str">
+      <c r="E24" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x002000</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="13"/>
       <c r="H24">
         <f t="shared" ref="H24:H27" si="11">+IF($E24&lt;&gt;"",HEX2DEC(RIGHT(E24,+LEN(E24)-2)),"")</f>
         <v>8192</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
+      <c r="A25" s="12" t="str">
         <f t="shared" si="7"/>
         <v>Loader</v>
       </c>
-      <c r="B25" s="6" t="str">
+      <c r="B25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>app</v>
       </c>
-      <c r="C25" s="6" t="str">
+      <c r="C25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota_0</v>
       </c>
-      <c r="D25" s="6" t="str">
+      <c r="D25" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x010000</v>
       </c>
-      <c r="E25" s="6" t="str">
+      <c r="E25" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x0F0000</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="13"/>
       <c r="H25">
         <f t="shared" si="11"/>
         <v>983040</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
+      <c r="A26" s="12" t="str">
         <f t="shared" si="7"/>
         <v>app</v>
       </c>
-      <c r="B26" s="6" t="str">
+      <c r="B26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>app</v>
       </c>
-      <c r="C26" s="6" t="str">
+      <c r="C26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota_1</v>
       </c>
-      <c r="D26" s="6" t="str">
+      <c r="D26" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x100000</v>
       </c>
-      <c r="E26" s="6" t="str">
+      <c r="E26" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x280000</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="13"/>
       <c r="H26">
         <f t="shared" si="11"/>
         <v>2621440</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
+      <c r="A27" s="12" t="str">
         <f t="shared" si="7"/>
         <v>spiffs</v>
       </c>
-      <c r="B27" s="6" t="str">
+      <c r="B27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>data</v>
       </c>
-      <c r="C27" s="6" t="str">
+      <c r="C27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>spiffs</v>
       </c>
-      <c r="D27" s="6" t="str">
+      <c r="D27" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x380000</v>
       </c>
-      <c r="E27" s="6" t="str">
+      <c r="E27" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x080000</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="13"/>
       <c r="H27">
         <f t="shared" si="11"/>
         <v>524288</v>
@@ -3016,27 +2928,27 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
+      <c r="A28" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="B28" s="6" t="str">
+      <c r="B28" s="5" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="C28" s="6" t="str">
+      <c r="C28" s="5" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D28" s="6" t="str">
+      <c r="D28" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E28" s="6" t="str">
+      <c r="E28" s="5" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="13"/>
       <c r="I28">
         <v>4096</v>
       </c>
@@ -3046,27 +2958,27 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="str">
+      <c r="A29" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="B29" s="16" t="str">
+      <c r="B29" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D29" s="16" t="str">
+      <c r="D29" s="15" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E29" s="16" t="str">
+      <c r="E29" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
       <c r="I29">
         <f>36+I13+I14+I16+I17</f>
         <v>3136</v>
@@ -3161,7 +3073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B43E6B0-5B54-428C-9D5E-D5F8106930A6}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -3172,22 +3084,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="P1" t="s">
@@ -3210,26 +3122,26 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="J2" s="55" t="s">
+      <c r="F2" s="11"/>
+      <c r="J2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="51" t="s">
         <v>72</v>
       </c>
       <c r="P2" t="s">
@@ -3252,29 +3164,29 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="I3" s="10" t="s">
+      <c r="F3" s="13"/>
+      <c r="I3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="53">
+      <c r="J3" s="48">
         <v>860246</v>
       </c>
-      <c r="K3" s="54">
+      <c r="K3" s="49">
         <f>+J3/J15</f>
         <v>0.48615971317997686</v>
       </c>
@@ -3298,29 +3210,29 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="I4" s="15" t="s">
+      <c r="F4" s="13"/>
+      <c r="I4" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <v>1288481</v>
       </c>
-      <c r="K4" s="52">
+      <c r="K4" s="47">
         <f>+J4/J16</f>
         <v>0.72817258481626157</v>
       </c>
@@ -3344,22 +3256,22 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="13"/>
       <c r="P5" t="s">
         <v>14</v>
       </c>
@@ -3380,22 +3292,22 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="13"/>
       <c r="P6" t="s">
         <v>18</v>
       </c>
@@ -3413,20 +3325,20 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S9">
@@ -3436,47 +3348,47 @@
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="60" t="s">
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="21" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="33" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="61"/>
+      <c r="J12" s="57"/>
       <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
@@ -3486,522 +3398,522 @@
       <c r="M12" t="s">
         <v>67</v>
       </c>
-      <c r="O12" s="39"/>
+      <c r="O12" s="35"/>
       <c r="P12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="str">
+      <c r="A13" s="9" t="str">
         <f t="shared" ref="A13:A19" si="0">IF(A2&lt;&gt;"",+A2,"")</f>
         <v>nvs</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <f t="shared" ref="B13:C19" si="1">+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(D2,+LEN(D2)-2)),"")</f>
         <v>36864</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <f t="shared" si="1"/>
         <v>20480</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <f>+IF($A13&lt;&gt;"",+B13+C13,"")</f>
         <v>57344</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="34">
         <f>+IF($E13&lt;&gt;"",+B13,"")</f>
         <v>36864</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="26">
         <f>+IF($E13&lt;&gt;"",+C13,"")/1024</f>
         <v>20</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="26">
         <f>+I13*1024</f>
         <v>20480</v>
       </c>
-      <c r="K13" s="41">
+      <c r="K13" s="36">
         <f>+IF($E13&lt;&gt;"",+H13+J13,"")</f>
         <v>57344</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="37">
         <f t="shared" ref="L13:L19" si="2">+J13/1024</f>
         <v>20</v>
       </c>
-      <c r="M13" s="42">
+      <c r="M13" s="37">
         <f t="shared" ref="M13:M19" si="3">+IF($E13&lt;&gt;"",($K$20-K13)/1024,"")</f>
         <v>4040</v>
       </c>
-      <c r="O13" s="18"/>
+      <c r="O13" s="17"/>
       <c r="P13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="str">
+      <c r="A14" s="12" t="str">
         <f t="shared" si="0"/>
         <v>otadata</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f t="shared" si="1"/>
         <v>57344</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f t="shared" si="1"/>
         <v>8192</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <f t="shared" ref="D14:D19" si="4">+IF($A14&lt;&gt;"",+B14+C14,"")</f>
         <v>65536</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="43">
+      <c r="H14" s="38">
         <f t="shared" ref="H14:H19" si="5">+IF($E14&lt;&gt;"",+K13,"")</f>
         <v>57344</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <f>+IF($E14&lt;&gt;"",+C14,"")/1024</f>
         <v>8</v>
       </c>
-      <c r="J14" s="26">
+      <c r="J14" s="25">
         <f>+I14*1024</f>
         <v>8192</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="39">
         <f t="shared" ref="K14:K19" si="6">+IF($E14&lt;&gt;"",+H14+J14,"")</f>
         <v>65536</v>
       </c>
-      <c r="L14" s="42">
+      <c r="L14" s="37">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="M14" s="42">
+      <c r="M14" s="37">
         <f t="shared" si="3"/>
         <v>4032</v>
       </c>
-      <c r="O14" s="45"/>
+      <c r="O14" s="40"/>
       <c r="P14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="str">
+      <c r="A15" s="12" t="str">
         <f t="shared" si="0"/>
         <v>app0</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <f t="shared" si="1"/>
         <v>917504</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <f t="shared" si="4"/>
         <v>983040</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="43">
+      <c r="H15" s="38">
         <f t="shared" si="5"/>
         <v>65536</v>
       </c>
-      <c r="I15" s="46">
+      <c r="I15" s="41">
         <f>27*64</f>
         <v>1728</v>
       </c>
-      <c r="J15" s="46">
+      <c r="J15" s="41">
         <f>+I15*1024</f>
         <v>1769472</v>
       </c>
-      <c r="K15" s="44">
+      <c r="K15" s="39">
         <f t="shared" si="6"/>
         <v>1835008</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="37">
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
-      <c r="M15" s="42">
+      <c r="M15" s="37">
         <f t="shared" si="3"/>
         <v>2304</v>
       </c>
-      <c r="O15" s="47"/>
+      <c r="O15" s="42"/>
       <c r="P15" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="12" t="str">
         <f t="shared" si="0"/>
         <v>app1</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f t="shared" si="1"/>
         <v>983040</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <f t="shared" si="1"/>
         <v>3160064</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <f t="shared" si="4"/>
         <v>4143104</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="43">
+      <c r="H16" s="38">
         <f t="shared" si="5"/>
         <v>1835008</v>
       </c>
-      <c r="I16" s="46">
+      <c r="I16" s="41">
         <f>27*64</f>
         <v>1728</v>
       </c>
-      <c r="J16" s="46">
+      <c r="J16" s="41">
         <f>+I16*1024</f>
         <v>1769472</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="39">
         <f t="shared" si="6"/>
         <v>3604480</v>
       </c>
-      <c r="L16" s="42">
+      <c r="L16" s="37">
         <f t="shared" si="2"/>
         <v>1728</v>
       </c>
-      <c r="M16" s="42">
+      <c r="M16" s="37">
         <f t="shared" si="3"/>
         <v>576</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="str">
+      <c r="A17" s="12" t="str">
         <f t="shared" si="0"/>
         <v>spiffs</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <f t="shared" si="1"/>
         <v>4143104</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <f t="shared" si="1"/>
         <v>51200</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <f t="shared" si="4"/>
         <v>4194304</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="43">
+      <c r="H17" s="38">
         <f t="shared" si="5"/>
         <v>3604480</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="41">
         <f>8*64</f>
         <v>512</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="41">
         <f>+I17*1024</f>
         <v>524288</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="39">
         <f t="shared" si="6"/>
         <v>4128768</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L17" s="37">
         <f t="shared" si="2"/>
         <v>512</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="37">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="str">
+      <c r="A18" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B18" s="6" t="str">
+      <c r="B18" s="5" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="5" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D18" s="24" t="str">
+      <c r="D18" s="23" t="str">
         <f>+IF($A18&lt;&gt;"",+B18+C18,"")</f>
         <v/>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="43" t="str">
+      <c r="E18" s="31"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="38" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="44" t="str">
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="39" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M18" s="42" t="str">
+      <c r="M18" s="37" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="str">
+      <c r="A19" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="B19" s="16" t="str">
+      <c r="B19" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C19" s="16" t="str">
+      <c r="C19" s="15" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D19" s="25" t="str">
+      <c r="D19" s="24" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="48" t="str">
+      <c r="E19" s="32"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="43" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="50" t="str">
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="L19" s="42">
+      <c r="L19" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M19" s="42" t="str">
+      <c r="M19" s="37" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="R19" s="19"/>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="51"/>
+      <c r="C20" s="46"/>
       <c r="K20" s="1">
         <f>4*1024*1024</f>
         <v>4194304</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="18">
         <f>SUM(L13:L19)+H13/1024</f>
         <v>4032</v>
       </c>
-      <c r="R20" s="19"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L21" s="19"/>
+      <c r="L21" s="18"/>
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="str">
+      <c r="A23" s="9" t="str">
         <f t="shared" ref="A23:A29" si="7">+IF(E13&lt;&gt;"",E13,"")</f>
         <v>nvs</v>
       </c>
-      <c r="B23" s="11" t="str">
+      <c r="B23" s="10" t="str">
         <f t="shared" ref="B23:C29" si="8">+IF($A23&lt;&gt;"",F13,"")</f>
         <v>data</v>
       </c>
-      <c r="C23" s="11" t="str">
+      <c r="C23" s="10" t="str">
         <f t="shared" si="8"/>
         <v>nvs</v>
       </c>
-      <c r="D23" s="11" t="str">
+      <c r="D23" s="10" t="str">
         <f t="shared" ref="D23:D29" si="9">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(H13,6)),"")</f>
         <v>0x009000</v>
       </c>
-      <c r="E23" s="11" t="str">
+      <c r="E23" s="10" t="str">
         <f t="shared" ref="E23:E29" si="10">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(J13,6)),"")</f>
         <v>0x005000</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="11"/>
       <c r="H23">
         <f>+IF($E23&lt;&gt;"",HEX2DEC(RIGHT(E23,+LEN(E23)-2)),"")</f>
         <v>20480</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="str">
+      <c r="A24" s="12" t="str">
         <f t="shared" si="7"/>
         <v>otadata</v>
       </c>
-      <c r="B24" s="6" t="str">
+      <c r="B24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>data</v>
       </c>
-      <c r="C24" s="6" t="str">
+      <c r="C24" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota</v>
       </c>
-      <c r="D24" s="6" t="str">
+      <c r="D24" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x00E000</v>
       </c>
-      <c r="E24" s="6" t="str">
+      <c r="E24" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x002000</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="13"/>
       <c r="H24">
         <f t="shared" ref="H24:H27" si="11">+IF($E24&lt;&gt;"",HEX2DEC(RIGHT(E24,+LEN(E24)-2)),"")</f>
         <v>8192</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
+      <c r="A25" s="12" t="str">
         <f t="shared" si="7"/>
         <v>Loader</v>
       </c>
-      <c r="B25" s="6" t="str">
+      <c r="B25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>app</v>
       </c>
-      <c r="C25" s="6" t="str">
+      <c r="C25" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota_0</v>
       </c>
-      <c r="D25" s="6" t="str">
+      <c r="D25" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x010000</v>
       </c>
-      <c r="E25" s="6" t="str">
+      <c r="E25" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x1B0000</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="13"/>
       <c r="H25">
         <f t="shared" si="11"/>
         <v>1769472</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
+      <c r="A26" s="12" t="str">
         <f t="shared" si="7"/>
         <v>app</v>
       </c>
-      <c r="B26" s="6" t="str">
+      <c r="B26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>app</v>
       </c>
-      <c r="C26" s="6" t="str">
+      <c r="C26" s="5" t="str">
         <f t="shared" si="8"/>
         <v>ota_1</v>
       </c>
-      <c r="D26" s="6" t="str">
+      <c r="D26" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x1C0000</v>
       </c>
-      <c r="E26" s="6" t="str">
+      <c r="E26" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x1B0000</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="13"/>
       <c r="H26">
         <f t="shared" si="11"/>
         <v>1769472</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
+      <c r="A27" s="12" t="str">
         <f t="shared" si="7"/>
         <v>spiffs</v>
       </c>
-      <c r="B27" s="6" t="str">
+      <c r="B27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>data</v>
       </c>
-      <c r="C27" s="6" t="str">
+      <c r="C27" s="5" t="str">
         <f t="shared" si="8"/>
         <v>spiffs</v>
       </c>
-      <c r="D27" s="6" t="str">
+      <c r="D27" s="5" t="str">
         <f t="shared" si="9"/>
         <v>0x370000</v>
       </c>
-      <c r="E27" s="6" t="str">
+      <c r="E27" s="5" t="str">
         <f t="shared" si="10"/>
         <v>0x080000</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="13"/>
       <c r="H27">
         <f t="shared" si="11"/>
         <v>524288</v>
@@ -4012,27 +3924,27 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
+      <c r="A28" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="B28" s="6" t="str">
+      <c r="B28" s="5" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="C28" s="6" t="str">
+      <c r="C28" s="5" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D28" s="6" t="str">
+      <c r="D28" s="5" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E28" s="6" t="str">
+      <c r="E28" s="5" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="13"/>
       <c r="I28">
         <v>4096</v>
       </c>
@@ -4042,27 +3954,27 @@
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="str">
+      <c r="A29" s="14" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="B29" s="16" t="str">
+      <c r="B29" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="C29" s="16" t="str">
+      <c r="C29" s="15" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="D29" s="16" t="str">
+      <c r="D29" s="15" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="E29" s="16" t="str">
+      <c r="E29" s="15" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
       <c r="I29">
         <f>36+I13+I14+I16+I17</f>
         <v>2304</v>
@@ -4137,6 +4049,1052 @@
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">, , , , , </v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="I12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9219555-470D-46DC-9E5C-187956077AD6}">
+  <dimension ref="A1:U40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="J2" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="I3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="48">
+        <v>860246</v>
+      </c>
+      <c r="K3" s="49">
+        <f>+J3/J15</f>
+        <v>0.48615971317997686</v>
+      </c>
+      <c r="P3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="I4" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1288481</v>
+      </c>
+      <c r="K4" s="47">
+        <f>+J4/J16</f>
+        <v>0.72817258481626157</v>
+      </c>
+      <c r="P4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" t="s">
+        <v>54</v>
+      </c>
+      <c r="T4" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="P5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" t="s">
+        <v>59</v>
+      </c>
+      <c r="T5" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <f>+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(S2,+LEN(D2)-2)),"")</f>
+        <v>36864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="57"/>
+      <c r="K12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M12" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" s="35"/>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="str">
+        <f t="shared" ref="A13:A19" si="0">IF(A2&lt;&gt;"",+A2,"")</f>
+        <v>nvs</v>
+      </c>
+      <c r="B13" s="10">
+        <f t="shared" ref="B13:C19" si="1">+IF($A13&lt;&gt;"",HEX2DEC(RIGHT(D2,+LEN(D2)-2)),"")</f>
+        <v>36864</v>
+      </c>
+      <c r="C13" s="10">
+        <f t="shared" si="1"/>
+        <v>20480</v>
+      </c>
+      <c r="D13" s="22">
+        <f>+IF($A13&lt;&gt;"",+B13+C13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="34">
+        <f>+IF($E13&lt;&gt;"",+B13,"")</f>
+        <v>36864</v>
+      </c>
+      <c r="I13" s="26">
+        <f>+IF($E13&lt;&gt;"",+C13,"")/1024</f>
+        <v>20</v>
+      </c>
+      <c r="J13" s="26">
+        <f t="shared" ref="J13:J18" si="2">+I13*1024</f>
+        <v>20480</v>
+      </c>
+      <c r="K13" s="36">
+        <f>+IF($E13&lt;&gt;"",+H13+J13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="L13" s="37">
+        <f t="shared" ref="L13:L19" si="3">+J13/1024</f>
+        <v>20</v>
+      </c>
+      <c r="M13" s="37">
+        <f t="shared" ref="M13:M19" si="4">+IF($E13&lt;&gt;"",($K$20-K13)/1024,"")</f>
+        <v>4040</v>
+      </c>
+      <c r="O13" s="17"/>
+      <c r="P13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>otadata</v>
+      </c>
+      <c r="B14" s="5">
+        <f t="shared" si="1"/>
+        <v>57344</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="1"/>
+        <v>8192</v>
+      </c>
+      <c r="D14" s="23">
+        <f t="shared" ref="D14:D19" si="5">+IF($A14&lt;&gt;"",+B14+C14,"")</f>
+        <v>65536</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="38">
+        <f t="shared" ref="H14:H19" si="6">+IF($E14&lt;&gt;"",+K13,"")</f>
+        <v>57344</v>
+      </c>
+      <c r="I14" s="25">
+        <f>+IF($E14&lt;&gt;"",+C14,"")/1024</f>
+        <v>8</v>
+      </c>
+      <c r="J14" s="25">
+        <f t="shared" si="2"/>
+        <v>8192</v>
+      </c>
+      <c r="K14" s="39">
+        <f t="shared" ref="K14:K19" si="7">+IF($E14&lt;&gt;"",+H14+J14,"")</f>
+        <v>65536</v>
+      </c>
+      <c r="L14" s="37">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="M14" s="37">
+        <f t="shared" si="4"/>
+        <v>4032</v>
+      </c>
+      <c r="O14" s="40"/>
+      <c r="P14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>app0</v>
+      </c>
+      <c r="B15" s="5">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="1"/>
+        <v>917504</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="5"/>
+        <v>983040</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="38">
+        <f t="shared" si="6"/>
+        <v>65536</v>
+      </c>
+      <c r="I15" s="41">
+        <f>27*64</f>
+        <v>1728</v>
+      </c>
+      <c r="J15" s="41">
+        <f t="shared" si="2"/>
+        <v>1769472</v>
+      </c>
+      <c r="K15" s="39">
+        <f t="shared" si="7"/>
+        <v>1835008</v>
+      </c>
+      <c r="L15" s="37">
+        <f t="shared" si="3"/>
+        <v>1728</v>
+      </c>
+      <c r="M15" s="37">
+        <f t="shared" si="4"/>
+        <v>2304</v>
+      </c>
+      <c r="O15" s="42"/>
+      <c r="P15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>app1</v>
+      </c>
+      <c r="B16" s="5">
+        <f t="shared" si="1"/>
+        <v>983040</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="1"/>
+        <v>3160064</v>
+      </c>
+      <c r="D16" s="23">
+        <f t="shared" si="5"/>
+        <v>4143104</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="38">
+        <f t="shared" si="6"/>
+        <v>1835008</v>
+      </c>
+      <c r="I16" s="41">
+        <f>27*64</f>
+        <v>1728</v>
+      </c>
+      <c r="J16" s="41">
+        <f t="shared" si="2"/>
+        <v>1769472</v>
+      </c>
+      <c r="K16" s="39">
+        <f t="shared" si="7"/>
+        <v>3604480</v>
+      </c>
+      <c r="L16" s="37">
+        <f t="shared" si="3"/>
+        <v>1728</v>
+      </c>
+      <c r="M16" s="37">
+        <f t="shared" si="4"/>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>spiffs</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" si="1"/>
+        <v>4143104</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="1"/>
+        <v>51200</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="5"/>
+        <v>4194304</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="38">
+        <f t="shared" si="6"/>
+        <v>3604480</v>
+      </c>
+      <c r="I17" s="41">
+        <f>8*64</f>
+        <v>512</v>
+      </c>
+      <c r="J17" s="41">
+        <f t="shared" si="2"/>
+        <v>524288</v>
+      </c>
+      <c r="K17" s="39">
+        <f t="shared" si="7"/>
+        <v>4128768</v>
+      </c>
+      <c r="L17" s="37">
+        <f t="shared" si="3"/>
+        <v>512</v>
+      </c>
+      <c r="M17" s="37">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B18" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D18" s="23" t="str">
+        <f>+IF($A18&lt;&gt;"",+B18+C18,"")</f>
+        <v/>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="38">
+        <f t="shared" si="6"/>
+        <v>4128768</v>
+      </c>
+      <c r="I18" s="41">
+        <f>1*64</f>
+        <v>64</v>
+      </c>
+      <c r="J18" s="41">
+        <f t="shared" si="2"/>
+        <v>65536</v>
+      </c>
+      <c r="K18" s="39">
+        <f t="shared" si="7"/>
+        <v>4194304</v>
+      </c>
+      <c r="L18" s="37">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="M18" s="37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D19" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="43" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="45" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L19" s="37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="37" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R19" s="18"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="46"/>
+      <c r="H20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" s="1">
+        <f>4*1024*1024</f>
+        <v>4194304</v>
+      </c>
+      <c r="L20" s="18">
+        <f>SUM(L13:L19)+H13/1024</f>
+        <v>4096</v>
+      </c>
+      <c r="R20" s="18"/>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>2126053</v>
+      </c>
+      <c r="I21">
+        <v>1419045</v>
+      </c>
+      <c r="J21" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21" s="18"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>+H21/1024</f>
+        <v>2076.2236328125</v>
+      </c>
+      <c r="I22">
+        <f>+I21/1024</f>
+        <v>1385.7861328125</v>
+      </c>
+      <c r="J22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="str">
+        <f t="shared" ref="A23:A29" si="8">+IF(E13&lt;&gt;"",E13,"")</f>
+        <v>nvs</v>
+      </c>
+      <c r="B23" s="10" t="str">
+        <f t="shared" ref="B23:C29" si="9">+IF($A23&lt;&gt;"",F13,"")</f>
+        <v>data</v>
+      </c>
+      <c r="C23" s="10" t="str">
+        <f t="shared" si="9"/>
+        <v>nvs</v>
+      </c>
+      <c r="D23" s="10" t="str">
+        <f t="shared" ref="D23:D29" si="10">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(H13,6)),"")</f>
+        <v>0x009000</v>
+      </c>
+      <c r="E23" s="10" t="str">
+        <f t="shared" ref="E23:E29" si="11">+IF($A23&lt;&gt;"",CONCATENATE("0x",DEC2HEX(J13,6)),"")</f>
+        <v>0x005000</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="H23">
+        <f>+H22-I16</f>
+        <v>348.2236328125</v>
+      </c>
+      <c r="I23">
+        <f>+I22-J16</f>
+        <v>-1768086.2138671875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>otadata</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>data</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>ota</v>
+      </c>
+      <c r="D24" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>0x00E000</v>
+      </c>
+      <c r="E24" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>0x002000</v>
+      </c>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>Loader</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>app</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>ota_0</v>
+      </c>
+      <c r="D25" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>0x010000</v>
+      </c>
+      <c r="E25" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>0x1B0000</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="H25">
+        <f>+I17-H23</f>
+        <v>163.7763671875</v>
+      </c>
+      <c r="I25">
+        <f>+I17-128</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>app</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>app</v>
+      </c>
+      <c r="C26" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>ota_1</v>
+      </c>
+      <c r="D26" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>0x1C0000</v>
+      </c>
+      <c r="E26" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>0x1B0000</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="H26">
+        <f>+H25*1024</f>
+        <v>167707</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>spiffs</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>data</v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>spiffs</v>
+      </c>
+      <c r="D27" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>0x370000</v>
+      </c>
+      <c r="E27" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>0x080000</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="N27">
+        <f>0.875*1024</f>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>coredump</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>data</v>
+      </c>
+      <c r="C28" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>coredump</v>
+      </c>
+      <c r="D28" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>0x3F0000</v>
+      </c>
+      <c r="E28" s="5" t="str">
+        <f t="shared" si="11"/>
+        <v>0x010000</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="I28">
+        <v>4096</v>
+      </c>
+      <c r="N28">
+        <f>900*1024</f>
+        <v>921600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="B29" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="C29" s="15" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="D29" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E29" s="15" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="I29">
+        <f>36+I13+I14+I16+I17</f>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>+I28-I29</f>
+        <v>1792</v>
+      </c>
+      <c r="K30">
+        <f>+I30</f>
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <f>+INT(K30/64)*64</f>
+        <v>1792</v>
+      </c>
+      <c r="L31">
+        <f>+K31+64</f>
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E32" t="e">
+        <f>+D25+E25</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>+CONCATENATE(A22,", ",B22,", ",C22,", ",D22,", ",E22,", ",F22)</f>
+        <v># Name, Type, SubType, Offset, Size, Flags</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" ref="A34:A40" si="12">+CONCATENATE(A23,", ",B23,", ",C23,", ",D23,", ",E23,", ",F23)</f>
+        <v xml:space="preserve">nvs, data, nvs, 0x009000, 0x005000, </v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">otadata, data, ota, 0x00E000, 0x002000, </v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">Loader, app, ota_0, 0x010000, 0x1B0000, </v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">app, app, ota_1, 0x1C0000, 0x1B0000, </v>
+      </c>
+      <c r="I37" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="J37" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" t="s">
+        <v>74</v>
+      </c>
+      <c r="M37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">spiffs, data, spiffs, 0x370000, 0x080000, </v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve">coredump, data, coredump, 0x3F0000, 0x010000, </v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f t="shared" si="12"/>
         <v xml:space="preserve">, , , , , </v>

</xml_diff>